<commit_message>
aggiornato n. 7 e 8
</commit_message>
<xml_diff>
--- a/university sql esercizi.xlsx
+++ b/university sql esercizi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katiepalumbo/Documents/Boolean/Assignments/db-university/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8794B0F7-C10A-464D-BEA7-B90F5113BCEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C7CE4E0-910D-ED44-BA49-26302AF58AA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16080" xr2:uid="{50FD12B5-0FA4-E040-BFAE-3463D45FB3C8}"/>
+    <workbookView xWindow="15400" yWindow="500" windowWidth="13020" windowHeight="16080" xr2:uid="{50FD12B5-0FA4-E040-BFAE-3463D45FB3C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <r>
       <t>SELECT</t>
@@ -1090,6 +1090,92 @@
         <family val="1"/>
       </rPr>
       <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>SELECT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF444444"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FFFF00FF"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF444444"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF770088"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>FROM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF444444"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF0055AA"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>`students`</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF444444"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF770088"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>WHERE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF444444"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t> TIMESTAMPDIFF(YEAR, `date_of_birth`, CURDATE())  &gt; 30;</t>
     </r>
   </si>
 </sst>
@@ -1224,7 +1310,7 @@
       <xdr:col>20</xdr:col>
       <xdr:colOff>393700</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1557,10 +1643,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A96B7C20-A188-E94E-9B7E-56CF8D51CB9A}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1590,50 +1676,55 @@
       </c>
     </row>
     <row r="4" spans="1:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>4</v>
-      </c>
       <c r="B4" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>8</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B13" s="2"/>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B14" s="2"/>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B20" s="2"/>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B21" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
join.txt complete (no bonus) - new name for query1
</commit_message>
<xml_diff>
--- a/university sql esercizi.xlsx
+++ b/university sql esercizi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katiepalumbo/Documents/Boolean/Assignments/db-university/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C7CE4E0-910D-ED44-BA49-26302AF58AA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B10B00AB-12EE-CF49-9D3B-383374AAF2CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15400" yWindow="500" windowWidth="13020" windowHeight="16080" xr2:uid="{50FD12B5-0FA4-E040-BFAE-3463D45FB3C8}"/>
   </bookViews>
@@ -258,7 +258,7 @@
         <rFont val="Courier New"/>
         <family val="1"/>
       </rPr>
-      <t>`teachers`</t>
+      <t>`degrees`</t>
     </r>
     <r>
       <rPr>
@@ -294,7 +294,7 @@
         <rFont val="Courier New"/>
         <family val="1"/>
       </rPr>
-      <t>`phone`</t>
+      <t>`name`</t>
     </r>
     <r>
       <rPr>
@@ -312,25 +312,25 @@
         <rFont val="Courier New"/>
         <family val="1"/>
       </rPr>
-      <t>IS</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <color rgb="FF444444"/>
-        <rFont val="Courier New"/>
-        <family val="1"/>
-      </rPr>
-      <t> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <color rgb="FF221199"/>
-        <rFont val="Courier New"/>
-        <family val="1"/>
-      </rPr>
-      <t>NULL</t>
+      <t>LIKE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF444444"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FFAA1111"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>'%magistrale%'</t>
     </r>
     <r>
       <rPr>
@@ -398,7 +398,7 @@
         <rFont val="Courier New"/>
         <family val="1"/>
       </rPr>
-      <t>`degrees`</t>
+      <t>`courses`</t>
     </r>
     <r>
       <rPr>
@@ -425,16 +425,25 @@
         <rFont val="Courier New"/>
         <family val="1"/>
       </rPr>
-      <t> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <color rgb="FF0055AA"/>
-        <rFont val="Courier New"/>
-        <family val="1"/>
-      </rPr>
-      <t>`name`</t>
+      <t> Period</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FFFF00FF"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FFAA1111"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>'I semestre'</t>
     </r>
     <r>
       <rPr>
@@ -452,16 +461,34 @@
         <rFont val="Courier New"/>
         <family val="1"/>
       </rPr>
-      <t>LIKE</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <color rgb="FF444444"/>
-        <rFont val="Courier New"/>
-        <family val="1"/>
-      </rPr>
-      <t> </t>
+      <t>AND</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF444444"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF235A81"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>Year</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FFFF00FF"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>=</t>
     </r>
     <r>
       <rPr>
@@ -470,7 +497,7 @@
         <rFont val="Courier New"/>
         <family val="1"/>
       </rPr>
-      <t>'%magistrale%'</t>
+      <t>'1'</t>
     </r>
     <r>
       <rPr>
@@ -538,7 +565,7 @@
         <rFont val="Courier New"/>
         <family val="1"/>
       </rPr>
-      <t>`courses`</t>
+      <t>`exams`</t>
     </r>
     <r>
       <rPr>
@@ -565,7 +592,16 @@
         <rFont val="Courier New"/>
         <family val="1"/>
       </rPr>
-      <t> Period</t>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF235A81"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>date</t>
     </r>
     <r>
       <rPr>
@@ -583,7 +619,7 @@
         <rFont val="Courier New"/>
         <family val="1"/>
       </rPr>
-      <t>'I semestre'</t>
+      <t>'2020-06-20'</t>
     </r>
     <r>
       <rPr>
@@ -610,16 +646,7 @@
         <rFont val="Courier New"/>
         <family val="1"/>
       </rPr>
-      <t> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <color rgb="FF235A81"/>
-        <rFont val="Courier New"/>
-        <family val="1"/>
-      </rPr>
-      <t>Year</t>
+      <t> hour </t>
     </r>
     <r>
       <rPr>
@@ -628,7 +655,16 @@
         <rFont val="Courier New"/>
         <family val="1"/>
       </rPr>
-      <t>=</t>
+      <t>&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF444444"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t> </t>
     </r>
     <r>
       <rPr>
@@ -637,7 +673,7 @@
         <rFont val="Courier New"/>
         <family val="1"/>
       </rPr>
-      <t>'1'</t>
+      <t>'14:00:00'</t>
     </r>
     <r>
       <rPr>
@@ -705,7 +741,7 @@
         <rFont val="Courier New"/>
         <family val="1"/>
       </rPr>
-      <t>`exams`</t>
+      <t>`courses`</t>
     </r>
     <r>
       <rPr>
@@ -732,88 +768,16 @@
         <rFont val="Courier New"/>
         <family val="1"/>
       </rPr>
-      <t> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <color rgb="FF235A81"/>
-        <rFont val="Courier New"/>
-        <family val="1"/>
-      </rPr>
-      <t>date</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <color rgb="FFFF00FF"/>
-        <rFont val="Courier New"/>
-        <family val="1"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <color rgb="FFAA1111"/>
-        <rFont val="Courier New"/>
-        <family val="1"/>
-      </rPr>
-      <t>'2020-06-20'</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <color rgb="FF444444"/>
-        <rFont val="Courier New"/>
-        <family val="1"/>
-      </rPr>
-      <t> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <color rgb="FF235A81"/>
-        <rFont val="Courier New"/>
-        <family val="1"/>
-      </rPr>
-      <t>AND</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <color rgb="FF444444"/>
-        <rFont val="Courier New"/>
-        <family val="1"/>
-      </rPr>
-      <t> hour </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <color rgb="FFFF00FF"/>
-        <rFont val="Courier New"/>
-        <family val="1"/>
-      </rPr>
-      <t>&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <color rgb="FF444444"/>
-        <rFont val="Courier New"/>
-        <family val="1"/>
-      </rPr>
-      <t> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <color rgb="FFAA1111"/>
-        <rFont val="Courier New"/>
-        <family val="1"/>
-      </rPr>
-      <t>'14:00:00'</t>
+      <t> cfu &gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF116644"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>10</t>
     </r>
     <r>
       <rPr>
@@ -881,7 +845,7 @@
         <rFont val="Courier New"/>
         <family val="1"/>
       </rPr>
-      <t>`courses`</t>
+      <t>`students`</t>
     </r>
     <r>
       <rPr>
@@ -908,7 +872,7 @@
         <rFont val="Courier New"/>
         <family val="1"/>
       </rPr>
-      <t> cfu &gt; </t>
+      <t> date_of_birth  &gt; '</t>
     </r>
     <r>
       <rPr>
@@ -917,7 +881,7 @@
         <rFont val="Courier New"/>
         <family val="1"/>
       </rPr>
-      <t>10</t>
+      <t>1992-03-21'</t>
     </r>
     <r>
       <rPr>
@@ -985,21 +949,39 @@
         <rFont val="Courier New"/>
         <family val="1"/>
       </rPr>
-      <t>`departments`;</t>
+      <t>`students`</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF444444"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF770088"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>WHERE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF444444"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t> TIMESTAMPDIFF(YEAR, `date_of_birth`, CURDATE())  &gt; 30;</t>
     </r>
   </si>
   <si>
     <r>
-      <t>SELECT</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <color rgb="FF444444"/>
-        <rFont val="Courier New"/>
-        <family val="1"/>
-      </rPr>
-      <t> </t>
+      <t>SELECT COUNT(</t>
     </r>
     <r>
       <rPr>
@@ -1008,7 +990,7 @@
         <rFont val="Courier New"/>
         <family val="1"/>
       </rPr>
-      <t>*</t>
+      <t>*)</t>
     </r>
     <r>
       <rPr>
@@ -1044,7 +1026,7 @@
         <rFont val="Courier New"/>
         <family val="1"/>
       </rPr>
-      <t>`students`</t>
+      <t>`teachers`</t>
     </r>
     <r>
       <rPr>
@@ -1071,16 +1053,52 @@
         <rFont val="Courier New"/>
         <family val="1"/>
       </rPr>
-      <t> date_of_birth  &gt; '</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <color rgb="FF116644"/>
-        <rFont val="Courier New"/>
-        <family val="1"/>
-      </rPr>
-      <t>1992-03-21'</t>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF0055AA"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>`phone`</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF444444"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF235A81"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>IS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF444444"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF221199"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>NULL</t>
     </r>
     <r>
       <rPr>
@@ -1103,7 +1121,7 @@
         <rFont val="Courier New"/>
         <family val="1"/>
       </rPr>
-      <t> </t>
+      <t> COUNT(</t>
     </r>
     <r>
       <rPr>
@@ -1112,7 +1130,7 @@
         <rFont val="Courier New"/>
         <family val="1"/>
       </rPr>
-      <t>*</t>
+      <t>*)</t>
     </r>
     <r>
       <rPr>
@@ -1148,34 +1166,7 @@
         <rFont val="Courier New"/>
         <family val="1"/>
       </rPr>
-      <t>`students`</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <color rgb="FF444444"/>
-        <rFont val="Courier New"/>
-        <family val="1"/>
-      </rPr>
-      <t> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <color rgb="FF770088"/>
-        <rFont val="Courier New"/>
-        <family val="1"/>
-      </rPr>
-      <t>WHERE</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <color rgb="FF444444"/>
-        <rFont val="Courier New"/>
-        <family val="1"/>
-      </rPr>
-      <t> TIMESTAMPDIFF(YEAR, `date_of_birth`, CURDATE())  &gt; 30;</t>
+      <t>`departments`;</t>
     </r>
   </si>
 </sst>
@@ -1646,7 +1637,7 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1664,7 +1655,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="18" x14ac:dyDescent="0.25">
@@ -1672,12 +1663,12 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="18" x14ac:dyDescent="0.25">
@@ -1685,7 +1676,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="18" x14ac:dyDescent="0.25">
@@ -1693,7 +1684,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="18" x14ac:dyDescent="0.25">
@@ -1701,7 +1692,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="18" x14ac:dyDescent="0.25">
@@ -1709,7 +1700,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="18" x14ac:dyDescent="0.25">
@@ -1717,7 +1708,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
updates after correzioni mattutine
</commit_message>
<xml_diff>
--- a/university sql esercizi.xlsx
+++ b/university sql esercizi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katiepalumbo/Documents/Boolean/Assignments/db-university/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B10B00AB-12EE-CF49-9D3B-383374AAF2CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BAF0707-918B-F44B-956D-6AE81A8027DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15400" yWindow="500" windowWidth="13020" windowHeight="16080" xr2:uid="{50FD12B5-0FA4-E040-BFAE-3463D45FB3C8}"/>
+    <workbookView xWindow="540" yWindow="500" windowWidth="27880" windowHeight="16080" xr2:uid="{50FD12B5-0FA4-E040-BFAE-3463D45FB3C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <r>
       <t>SELECT</t>
@@ -1167,6 +1167,982 @@
         <family val="1"/>
       </rPr>
       <t>`departments`;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SELECT </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FFFF00FF"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF444444"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF770088"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>FROM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF444444"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF0055AA"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>`students`</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF444444"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> join `degrees` ON `students`.`degree_id` = `degrees`.`id` </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF770088"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>WHERE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF444444"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF0055AA"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>`degrees`.`name` = 'Corso di Laurea in Economia'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF444444"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <t>SELECT * FROM `degrees` JOIN `departments` ON `degrees`.`department_id` = `departments`.`id` WHERE `departments`.`name` = 'Dipartimento di Neuroscienze';</t>
+  </si>
+  <si>
+    <t>SELECT * FROM `courses` JOIN `course_teacher` ON `courses`.`id` = `course_teacher`.`course_id` WHERE `course_teacher`.`teacher_id` = 44;</t>
+  </si>
+  <si>
+    <t>SELECT * FROM `students` JOIN `degrees` ON `students`.`degree_id` = `degrees`.`id` JOIN `departments` ON `degrees`.`department_id` = `departments`.`id` ORDER BY `students`.`surname`, `students`.`name`;</t>
+  </si>
+  <si>
+    <t>SELECT `degrees`.`name`, `teachers`.`name`, `teachers`.`surname`,`courses`.`name` FROM `degrees` JOIN `courses` ON `courses`.`degree_id` = `degrees`.`id` JOIN `course_teacher` ON `course_teacher`.`course_id` = `courses`.`id` JOIN `teachers` on `course_teacher`.`teacher_id` = `teachers`.`id`;</t>
+  </si>
+  <si>
+    <t>SELECT DISTINCT `teachers`.`name`, `teachers`.`surname` FROM `departments` JOIN `degrees` on `degrees`.`department_id` = `departments`.`id` JOIN `courses` on `courses`.`degree_id` = `degrees`.`id` JOIN `course_teacher` on `course_teacher`.`course_id` = `courses`.`id` JOIN `teachers` on `course_teacher`.`teacher_id` = `teachers`.`id` WHERE `departments`.`id` = 5 ORDER BY `teachers`.`surname` ASC;</t>
+  </si>
+  <si>
+    <r>
+      <t>SELECT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF444444"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t> EXTRACT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF999977"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF235A81"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>year</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF444444"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF770088"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>FROM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF444444"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t> enrolment_date</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF999977"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF444444"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF770088"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>AS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF444444"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF235A81"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>year</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF444444"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF235A81"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>COUNT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF999977"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FFFF00FF"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF999977"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF444444"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF770088"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>AS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF444444"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t> students_enrolled </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF770088"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>FROM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF444444"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF0055AA"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>`students`</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF444444"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF770088"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>GROUP</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF444444"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF770088"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>BY</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF444444"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t> EXTRACT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF999977"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF235A81"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>year</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF444444"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF770088"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>FROM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF444444"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t> enrolment_date</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF999977"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF444444"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>SELECT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF444444"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF235A81"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>COUNT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF999977"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FFFF00FF"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF999977"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF444444"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF770088"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>AS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF444444"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FFAA1111"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>'teachers_same_office'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF444444"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF0055AA"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>`office_address`</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF444444"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF770088"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>FROM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF444444"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF0055AA"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>`teachers`</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF444444"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF770088"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>GROUP</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF444444"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF770088"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>BY</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF444444"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF0055AA"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>`office_address`</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF444444"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>SELECT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF444444"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF0055AA"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>`exam_id`</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF444444"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF770088"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>as</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF444444"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t> exam_id, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF235A81"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>AVG</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF999977"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF0055AA"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>`vote`</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF999977"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF444444"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF770088"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>AS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF444444"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t> avg_grade </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF770088"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>FROM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF444444"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF0055AA"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>`exam_student`</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF444444"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF770088"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>group</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF444444"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF770088"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>by</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF444444"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF0055AA"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>`exam_id`</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF444444"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>select</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF444444"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t> department_id </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF770088"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>as</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF444444"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t> department_id, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF235A81"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>COUNT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF999977"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF444444"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF999977"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF444444"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF770088"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>as</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF444444"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t> number_of_degrees </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF770088"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>from</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF444444"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t> degrees </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF770088"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>group</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF444444"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF770088"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>by</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF444444"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t> department_id;</t>
     </r>
   </si>
 </sst>
@@ -1326,6 +2302,94 @@
         <a:xfrm>
           <a:off x="9906000" y="228600"/>
           <a:ext cx="6172200" cy="3924300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>539882</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>711200</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{05D5E4B2-88DB-7D42-8B76-B5AC70305E7A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11271382" y="5651500"/>
+          <a:ext cx="5124318" cy="2882900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>83227</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE57FCD2-991C-7D46-8F9C-4AC0DBB264BF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11264900" y="8801100"/>
+          <a:ext cx="4432300" cy="2204127"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1634,10 +2698,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A96B7C20-A188-E94E-9B7E-56CF8D51CB9A}">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1714,11 +2778,100 @@
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B14" s="2"/>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B21" s="2"/>
     </row>
+    <row r="23" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>2</v>
+      </c>
+      <c r="B24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>3</v>
+      </c>
+      <c r="B25" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>4</v>
+      </c>
+      <c r="B26" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>5</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>6</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>1</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>2</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>3</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>4</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B27" r:id="rId1" display="http://localhost/phpMyAdmin5/url.php?url=https://dev.mysql.com/doc/refman/5.7/en/select.html" xr:uid="{30EEA3E3-6CF8-224C-BD02-6BA3A455F65F}"/>
+    <hyperlink ref="B28" r:id="rId2" display="http://localhost/phpMyAdmin5/url.php?url=https://dev.mysql.com/doc/refman/5.7/en/select.html" xr:uid="{4C80AF1F-DF2C-164E-BDDE-0A6AABF5A7CD}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>